<commit_message>
Iter 10. Homework complete.
</commit_message>
<xml_diff>
--- a/logs/hw04-GC/statlog_TMPL.xlsx
+++ b/logs/hw04-GC/statlog_TMPL.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20367"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\java\otus-java-2020-09\logs\hw04-GC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38890A3F-6C64-43A5-8349-D9C0F2628AAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="22065" windowHeight="9630"/>
+    <workbookView xWindow="5205" yWindow="0" windowWidth="22065" windowHeight="9630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="statlog_TMPL" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="20">
   <si>
     <t>application starts at 12:03:42.274</t>
   </si>
@@ -70,12 +71,21 @@
   </si>
   <si>
     <t>median GC durations</t>
+  </si>
+  <si>
+    <t>sec</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>Throughput</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -571,9 +581,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -894,11 +907,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,6 +1488,10 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>A21+B21+D21</f>
+        <v>10188</v>
+      </c>
       <c r="B22">
         <f>SUM(B3:B21)</f>
         <v>8170</v>
@@ -1485,12 +1502,22 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="D23">
-        <f>D22/B22</f>
-        <v>0.24687882496940025</v>
+        <f>1-D22/A22</f>
+        <v>0.80202198665096192</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>A21/1000</f>
+        <v>9.9060000000000006</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
       <c r="D25" s="1">
         <f>MAX(D3:D21)</f>
         <v>367</v>
@@ -1500,6 +1527,13 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f>TRUNC(A25/60)</f>
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
       <c r="D26" s="1">
         <f>AVERAGE(D3:D21)</f>
         <v>106.15789473684211</v>
@@ -1509,6 +1543,13 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <f>MOD(A25,60)</f>
+        <v>9.9060000000000006</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
       <c r="D27">
         <f>MEDIAN(D3:D21)</f>
         <v>40</v>

</xml_diff>